<commit_message>
one more data needed
</commit_message>
<xml_diff>
--- a/dataneeded.xlsx
+++ b/dataneeded.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Basic Information</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>P.S. While dealing with QS and THE World University Rankings, we need to extract colleges in the US and record their international ranking, then sort nationally.</t>
+  </si>
+  <si>
+    <t>SAT/ACT scores must be received by</t>
   </si>
 </sst>
 </file>
@@ -523,7 +526,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,10 +576,13 @@
       <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>